<commit_message>
Finalisation des données excel pour cette revue
</commit_message>
<xml_diff>
--- a/Revue de projet/Tableau et graphiques des heures.xlsx
+++ b/Revue de projet/Tableau et graphiques des heures.xlsx
@@ -8,18 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BUT 3 Temp\s5.a.01-developpement-avance\Revue de projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB08095-9F89-4A53-B2D9-150357598604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6716A57-01F2-4A92-AF6D-727610D90B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{BCEF3A41-EA7E-4D58-AA60-0E9BF84A5E38}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau" sheetId="1" r:id="rId1"/>
     <sheet name="Graphique" sheetId="4" r:id="rId2"/>
-    <sheet name="Graphique 2" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId4"/>
+    <pivotCache cacheId="13" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="131">
   <si>
     <t xml:space="preserve"> Nombre d'heures </t>
   </si>
@@ -362,15 +361,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FIN DE L'API                     </t>
-  </si>
-  <si>
-    <t>FIN DE L'API                    </t>
-  </si>
-  <si>
-    <t> </t>
   </si>
   <si>
     <r>
@@ -458,31 +448,22 @@
     <t>Les "+1" dans les formules sont pour le temps passer en veille numérique durant tout le projet</t>
   </si>
   <si>
-    <t>Document de suivis de projet</t>
-  </si>
-  <si>
-    <t>Base de données</t>
-  </si>
-  <si>
-    <t>Développement de l'API</t>
-  </si>
-  <si>
-    <t>Développement de l'application web</t>
-  </si>
-  <si>
-    <t>CI/CD</t>
-  </si>
-  <si>
-    <t>Veille numérique</t>
-  </si>
-  <si>
     <t>Initialisation du projet</t>
   </si>
   <si>
     <t xml:space="preserve">Initialisation du projet </t>
   </si>
   <si>
-    <t>Revue de projet</t>
+    <t>Finalisation du diaporama</t>
+  </si>
+  <si>
+    <t>Correction de quelque diagramme et des fautes d'orthographe</t>
+  </si>
+  <si>
+    <t>Finalisation du rapport technique</t>
+  </si>
+  <si>
+    <t>Finalisation des dernières précision et correction des fautes d'orthographe</t>
   </si>
 </sst>
 </file>
@@ -517,18 +498,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -563,13 +538,13 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1815,6 +1790,746 @@
           </c:extLst>
         </c:dLbl>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="14"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="15"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="16"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="17"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="18"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="19"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="20"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="21"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="22"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="23"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="24"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="25"/>
+        <c:spPr>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -1827,7 +2542,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Graphique!$B$1</c:f>
+              <c:f>Graphique!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1933,7 +2648,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Graphique!$A$2:$A$13</c:f>
+              <c:f>Graphique!$A$4:$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -1974,7 +2689,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Graphique!$B$2:$B$13</c:f>
+              <c:f>Graphique!$B$4:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1997,7 +2712,7 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>24.5</c:v>
+                  <c:v>27.75</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1</c:v>
@@ -2901,7 +3616,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Loïc SERRE" refreshedDate="45334.993143287036" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="11" xr:uid="{37BD6C46-9FB5-43AA-B54A-02B37C8F268B}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Loïc SERRE" refreshedDate="45335.850467939817" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="11" xr:uid="{37BD6C46-9FB5-43AA-B54A-02B37C8F268B}">
   <cacheSource type="worksheet">
     <worksheetSource ref="H1:J12" sheet="Tableau"/>
   </cacheSource>
@@ -2910,7 +3625,19 @@
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1" maxValue="37.5"/>
     </cacheField>
     <cacheField name="Semaine n°" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="52"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="52" count="11">
+        <n v="49"/>
+        <n v="50"/>
+        <n v="51"/>
+        <n v="52"/>
+        <n v="1"/>
+        <n v="2"/>
+        <n v="3"/>
+        <n v="4"/>
+        <n v="5"/>
+        <n v="6"/>
+        <n v="7"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Mois" numFmtId="17">
       <sharedItems count="11">
@@ -2940,68 +3667,83 @@
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="11">
   <r>
     <n v="3"/>
-    <n v="49"/>
+    <x v="0"/>
     <x v="0"/>
   </r>
   <r>
     <n v="15.75"/>
-    <n v="50"/>
+    <x v="1"/>
     <x v="1"/>
   </r>
   <r>
     <n v="6.25"/>
-    <n v="51"/>
+    <x v="2"/>
     <x v="2"/>
   </r>
   <r>
     <n v="37"/>
-    <n v="52"/>
+    <x v="3"/>
     <x v="3"/>
   </r>
   <r>
     <n v="1"/>
-    <n v="1"/>
+    <x v="4"/>
     <x v="4"/>
   </r>
   <r>
     <n v="2"/>
-    <n v="2"/>
+    <x v="5"/>
     <x v="5"/>
   </r>
   <r>
     <n v="37.5"/>
-    <n v="3"/>
+    <x v="6"/>
     <x v="6"/>
   </r>
   <r>
     <n v="8"/>
-    <n v="4"/>
+    <x v="7"/>
     <x v="7"/>
   </r>
   <r>
     <n v="2.5"/>
-    <n v="5"/>
+    <x v="8"/>
     <x v="8"/>
   </r>
   <r>
     <n v="19"/>
-    <n v="6"/>
+    <x v="9"/>
     <x v="9"/>
   </r>
   <r>
-    <n v="24.5"/>
-    <n v="7"/>
+    <n v="27.75"/>
+    <x v="10"/>
     <x v="10"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6F07C3AD-D351-4504-9CFE-BD7B5982BEA1}" name="Tableau croisé dynamique23" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
-  <location ref="A1:B13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6F07C3AD-D351-4504-9CFE-BD7B5982BEA1}" name="Tableau croisé dynamique23" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="A3:B15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="12">
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField axis="axisRow" showAll="0">
       <items count="12">
         <item x="0"/>
@@ -3386,10 +4128,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E521F19A-36BD-4570-A65D-125F4D2EFE77}">
-  <dimension ref="A1:J78"/>
+  <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71:D78"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3408,29 +4150,29 @@
   <sheetData>
     <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="B1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>112</v>
+      <c r="J1" s="5" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -3443,8 +4185,8 @@
       <c r="I2">
         <v>49</v>
       </c>
-      <c r="J2" s="9" t="s">
-        <v>120</v>
+      <c r="J2" s="8" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -3472,8 +4214,8 @@
       <c r="I3">
         <v>50</v>
       </c>
-      <c r="J3" s="9" t="s">
-        <v>121</v>
+      <c r="J3" s="8" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -3501,8 +4243,8 @@
       <c r="I4">
         <v>51</v>
       </c>
-      <c r="J4" s="9" t="s">
-        <v>122</v>
+      <c r="J4" s="8" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -3530,8 +4272,8 @@
       <c r="I5">
         <v>52</v>
       </c>
-      <c r="J5" s="9" t="s">
-        <v>123</v>
+      <c r="J5" s="8" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -3558,8 +4300,8 @@
       <c r="I6">
         <v>1</v>
       </c>
-      <c r="J6" s="9" t="s">
-        <v>116</v>
+      <c r="J6" s="8" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -3586,8 +4328,8 @@
       <c r="I7">
         <v>2</v>
       </c>
-      <c r="J7" s="9" t="s">
-        <v>117</v>
+      <c r="J7" s="8" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -3615,8 +4357,8 @@
       <c r="I8">
         <v>3</v>
       </c>
-      <c r="J8" s="9" t="s">
-        <v>118</v>
+      <c r="J8" s="8" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -3644,8 +4386,8 @@
       <c r="I9">
         <v>4</v>
       </c>
-      <c r="J9" s="9" t="s">
-        <v>119</v>
+      <c r="J9" s="8" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -3673,8 +4415,8 @@
       <c r="I10">
         <v>5</v>
       </c>
-      <c r="J10" s="9" t="s">
-        <v>124</v>
+      <c r="J10" s="8" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -3702,8 +4444,8 @@
       <c r="I11">
         <v>6</v>
       </c>
-      <c r="J11" s="9" t="s">
-        <v>125</v>
+      <c r="J11" s="8" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -3725,14 +4467,14 @@
         <v>50</v>
       </c>
       <c r="H12">
-        <f>SUM(E59:E65)</f>
-        <v>24.5</v>
+        <f>SUM(E59:E67)</f>
+        <v>27.75</v>
       </c>
       <c r="I12">
         <v>7</v>
       </c>
-      <c r="J12" s="9" t="s">
-        <v>126</v>
+      <c r="J12" s="8" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -3757,10 +4499,10 @@
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C14" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D14" s="2">
         <v>45274</v>
@@ -3792,7 +4534,7 @@
         <v>50</v>
       </c>
       <c r="H15" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -4190,7 +4932,7 @@
         <v>3.5</v>
       </c>
       <c r="F36">
-        <f t="shared" ref="F36:F65" si="1">WEEKNUM(D36,1)</f>
+        <f t="shared" ref="F36:F67" si="1">WEEKNUM(D36,1)</f>
         <v>52</v>
       </c>
     </row>
@@ -4747,99 +5489,60 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
+      <c r="B66" t="s">
+        <v>127</v>
+      </c>
       <c r="C66" t="s">
-        <v>42</v>
-      </c>
-      <c r="D66" s="2"/>
+        <v>128</v>
+      </c>
+      <c r="D66" s="2">
+        <v>45335</v>
+      </c>
+      <c r="E66">
+        <v>1.25</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" t="s">
-        <v>41</v>
+        <v>129</v>
       </c>
       <c r="C67" t="s">
-        <v>42</v>
-      </c>
-      <c r="D67" t="s">
-        <v>43</v>
+        <v>130</v>
+      </c>
+      <c r="D67" s="2">
+        <v>45335</v>
+      </c>
+      <c r="E67">
+        <v>2</v>
+      </c>
+      <c r="F67">
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
-      <c r="B68" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="E68" s="3"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C71" t="s">
-        <v>134</v>
-      </c>
-      <c r="D71">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C72" t="s">
-        <v>128</v>
-      </c>
-      <c r="D72">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C73" t="s">
-        <v>129</v>
-      </c>
-      <c r="D73">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C74" t="s">
-        <v>130</v>
-      </c>
-      <c r="D74">
-        <v>25.25</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C75" t="s">
-        <v>131</v>
-      </c>
-      <c r="D75">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C76" t="s">
-        <v>132</v>
-      </c>
-      <c r="D76">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C77" t="s">
-        <v>133</v>
-      </c>
-      <c r="D77">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C78" t="s">
-        <v>136</v>
-      </c>
-      <c r="D78">
-        <v>20.5</v>
-      </c>
+      <c r="B68" t="s">
+        <v>41</v>
+      </c>
+      <c r="C68" t="s">
+        <v>42</v>
+      </c>
+      <c r="D68" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="1"/>
+      <c r="B69" s="9"/>
+      <c r="C69" s="9"/>
+      <c r="D69" s="9"/>
+      <c r="E69" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -4850,10 +5553,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DC8A0C5-9B37-4AA8-BC1B-5DEE4931DF96}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A3:B15"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4861,135 +5564,124 @@
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" s="10">
+        <v>15.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="10">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" s="10">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" s="10">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" s="10">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" s="10">
+        <v>27.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="B2" s="10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="B3" s="10">
-        <v>15.75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="B4" s="10">
-        <v>6.25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="B5" s="10">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="B6" s="10">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="B7" s="10">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="B8" s="10">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="B12" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" s="10">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B9" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="B10" s="10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B11" s="10">
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="B12" s="10">
+      <c r="B14" s="10">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="B13" s="10">
-        <v>156.5</v>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B15" s="10">
+        <v>159.75</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D8A113D-3A82-4986-9E5A-43AA399C1484}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>